<commit_message>
Now time to probe the algorithm
</commit_message>
<xml_diff>
--- a/CH-80 Convex Hulls.xlsx
+++ b/CH-80 Convex Hulls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947AE5FF-D9C8-44D9-A2F4-118799E16689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE58577F-12F0-4DA4-BC6C-BA75AD160CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
   <si>
     <t>X</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Resul: Points on the convex Are Vertexes</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7216546666877739008/</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -333,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6630,8 +6636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6669,6 +6675,9 @@
       </c>
       <c r="F2" s="20" t="s">
         <v>1</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8521,8 +8530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC599161-5475-4CF5-9B5C-D6CD190124F7}">
   <dimension ref="B1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>